<commit_message>
Renomeando o projeto e corrigindo besteira
</commit_message>
<xml_diff>
--- a/resources/sourcedata/origem2.xlsx
+++ b/resources/sourcedata/origem2.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="98">
   <si>
     <t>order-id</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>573.382.250-36</t>
+  </si>
+  <si>
+    <t>Dave Harley Petterson</t>
+  </si>
+  <si>
+    <t>daveharleypetterson02@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -507,6 +513,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -797,7 +806,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +815,7 @@
     <col min="2" max="2" width="13.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="20" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" style="20" customWidth="1"/>
     <col min="7" max="7" width="14" style="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" style="20" bestFit="1" customWidth="1"/>
@@ -1737,11 +1746,11 @@
       <c r="D15" s="12">
         <v>45427</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>35</v>
+      <c r="E15" s="33" t="s">
+        <v>97</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>92</v>
@@ -1801,11 +1810,11 @@
       <c r="D16" s="12">
         <v>45427</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>35</v>
+      <c r="E16" s="33" t="s">
+        <v>97</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>92</v>
@@ -1865,11 +1874,11 @@
       <c r="D17" s="12">
         <v>45427</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>35</v>
+      <c r="E17" s="33" t="s">
+        <v>97</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>92</v>
@@ -2692,8 +2701,10 @@
     <hyperlink ref="E13:E14" r:id="rId4" display="marcosalmeidajonas@gmail.com"/>
     <hyperlink ref="E9" r:id="rId5"/>
     <hyperlink ref="E10:E11" r:id="rId6" display="janainacorrea@hotmail.com"/>
+    <hyperlink ref="E15" r:id="rId7"/>
+    <hyperlink ref="E16:E17" r:id="rId8" display="daveharleypetterson02@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="5" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="5" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>